<commit_message>
Aspects update (to be merged manually)
</commit_message>
<xml_diff>
--- a/groove/branches/aspects/src/meta/aspects.xlsx
+++ b/groove/branches/aspects/src/meta/aspects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2022-09\aspects\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace-2023-03\aspects\src\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388B80DF-ADC1-4AF0-8046-7A45B79DCFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9E57AB-8B94-48E0-953A-4BB64E5BD2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24720" yWindow="2580" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Category usage" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="46">
   <si>
     <t>ROLE</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>MULT_I-</t>
+  </si>
+  <si>
+    <t>c7</t>
+  </si>
+  <si>
+    <t>c1 but for assignments, which are only for readers and creators</t>
   </si>
 </sst>
 </file>
@@ -684,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +700,7 @@
     <col min="2" max="9" width="6.140625" customWidth="1"/>
     <col min="10" max="10" width="6.140625" style="4" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="17" width="6.140625" customWidth="1"/>
+    <col min="12" max="18" width="6.140625" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="2"/>
     <col min="20" max="20" width="9.140625" style="11"/>
   </cols>
@@ -1728,6 +1734,12 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
+      <c r="S35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T35" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1823,12 +1835,15 @@
         <v>5</v>
       </c>
       <c r="O39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P39" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q39" s="3" t="s">
+      <c r="R39" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1865,13 +1880,16 @@
       <c r="N40" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="O40" s="6" t="s">
         <v>33</v>
       </c>
       <c r="P40" s="2" t="s">
         <v>33</v>
       </c>
       <c r="Q40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R40" s="2" t="s">
         <v>33</v>
       </c>
       <c r="S40" s="2" t="s">
@@ -1916,13 +1934,16 @@
       <c r="N41" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q41" s="2" t="s">
+      <c r="O41" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R41" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1969,7 +1990,10 @@
       <c r="P42" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q42" s="2" t="s">
+      <c r="Q42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R42" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2000,7 +2024,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="5"/>
       <c r="K43" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="L43" s="5" t="str">
         <f>O40</f>
@@ -2019,7 +2043,10 @@
         <v>18</v>
       </c>
       <c r="Q43" s="6" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -2050,7 +2077,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="5"/>
       <c r="K44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L44" s="5" t="str">
         <f>P40</f>
@@ -2058,7 +2085,7 @@
       </c>
       <c r="M44" s="5" t="str">
         <f>P41</f>
-        <v>X</v>
+        <v>-</v>
       </c>
       <c r="N44" s="5" t="str">
         <f>P42</f>
@@ -2071,6 +2098,9 @@
       <c r="P44" s="7"/>
       <c r="Q44" s="6" t="s">
         <v>18</v>
+      </c>
+      <c r="R44" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -2102,7 +2132,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="5"/>
       <c r="K45" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="L45" s="5" t="str">
         <f>Q40</f>
@@ -2110,7 +2140,7 @@
       </c>
       <c r="M45" s="5" t="str">
         <f>Q41</f>
-        <v>-</v>
+        <v>X</v>
       </c>
       <c r="N45" s="5" t="str">
         <f>Q42</f>
@@ -2118,13 +2148,16 @@
       </c>
       <c r="O45" s="5" t="str">
         <f>Q43</f>
-        <v>c1</v>
+        <v>X</v>
       </c>
       <c r="P45" s="5" t="str">
         <f>Q44</f>
         <v>X</v>
       </c>
       <c r="Q45" s="7"/>
+      <c r="R45" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
@@ -2136,12 +2169,34 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="5"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
+      <c r="K46" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" s="5" t="str">
+        <f>R40</f>
+        <v>-</v>
+      </c>
+      <c r="M46" s="5" t="str">
+        <f>R41</f>
+        <v>-</v>
+      </c>
+      <c r="N46" s="5" t="str">
+        <f>R42</f>
+        <v>X</v>
+      </c>
+      <c r="O46" s="5" t="str">
+        <f>R43</f>
+        <v>X</v>
+      </c>
+      <c r="P46" s="5" t="str">
+        <f>R44</f>
+        <v>c1</v>
+      </c>
+      <c r="Q46" s="5" t="str">
+        <f>R45</f>
+        <v>X</v>
+      </c>
+      <c r="R46" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>